<commit_message>
chore: Added dependencies in requirements.txt
</commit_message>
<xml_diff>
--- a/optimized_portfolio.xlsx
+++ b/optimized_portfolio.xlsx
@@ -465,13 +465,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2007</v>
+        <v>0.2061</v>
       </c>
       <c r="C2" t="n">
-        <v>100350</v>
+        <v>103030</v>
       </c>
       <c r="D2" t="n">
-        <v>2795</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="3">
@@ -481,13 +481,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1982</v>
+        <v>0.1843</v>
       </c>
       <c r="C3" t="n">
-        <v>99080</v>
+        <v>92160</v>
       </c>
       <c r="D3" t="n">
-        <v>8616</v>
+        <v>8014</v>
       </c>
     </row>
     <row r="4">
@@ -497,13 +497,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2003</v>
+        <v>0.2024</v>
       </c>
       <c r="C4" t="n">
-        <v>100135</v>
+        <v>101210</v>
       </c>
       <c r="D4" t="n">
-        <v>1247</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="5">
@@ -513,13 +513,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1994</v>
+        <v>0.1945</v>
       </c>
       <c r="C5" t="n">
-        <v>99675</v>
+        <v>97255</v>
       </c>
       <c r="D5" t="n">
-        <v>3029</v>
+        <v>2955</v>
       </c>
     </row>
     <row r="6">
@@ -529,13 +529,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2015</v>
+        <v>0.2127</v>
       </c>
       <c r="C6" t="n">
-        <v>100760</v>
+        <v>106350</v>
       </c>
       <c r="D6" t="n">
-        <v>100760</v>
+        <v>106350</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0672027224617542</v>
+        <v>0.06765256308685724</v>
       </c>
     </row>
     <row r="3">
@@ -586,7 +586,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3555742737383193</v>
+        <v>0.3542435047398688</v>
       </c>
     </row>
     <row r="4">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1327506682794844</v>
+        <v>0.1345192288616552</v>
       </c>
     </row>
   </sheetData>
@@ -647,13 +647,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3324</v>
+        <v>0.3432</v>
       </c>
       <c r="C2" t="n">
-        <v>166175</v>
+        <v>171585</v>
       </c>
       <c r="D2" t="n">
-        <v>4629</v>
+        <v>4780</v>
       </c>
     </row>
     <row r="3">
@@ -663,13 +663,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0587</v>
+        <v>0.0313</v>
       </c>
       <c r="C3" t="n">
-        <v>29335</v>
+        <v>15650</v>
       </c>
       <c r="D3" t="n">
-        <v>2551</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="4">
@@ -679,13 +679,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2595</v>
+        <v>0.2641</v>
       </c>
       <c r="C4" t="n">
-        <v>129740</v>
+        <v>132050</v>
       </c>
       <c r="D4" t="n">
-        <v>1615</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="5">
@@ -695,13 +695,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.213</v>
+        <v>0.204</v>
       </c>
       <c r="C5" t="n">
-        <v>106485</v>
+        <v>101980</v>
       </c>
       <c r="D5" t="n">
-        <v>3236</v>
+        <v>3099</v>
       </c>
     </row>
     <row r="6">
@@ -711,13 +711,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1365</v>
+        <v>0.1575</v>
       </c>
       <c r="C6" t="n">
-        <v>68270</v>
+        <v>78735</v>
       </c>
       <c r="D6" t="n">
-        <v>68270</v>
+        <v>78735</v>
       </c>
     </row>
   </sheetData>
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.07765344505703034</v>
+        <v>0.07857468323672587</v>
       </c>
     </row>
     <row r="3">
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3933233338568988</v>
+        <v>0.3949529727706366</v>
       </c>
     </row>
     <row r="4">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1465802816519555</v>
+        <v>0.1483079943057987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>